<commit_message>
added the business explanation doc prepared by Nitesh
</commit_message>
<xml_diff>
--- a/data/ETL-Replacement/Safeway Customer Order Import.TMS 12_06.xlsx
+++ b/data/ETL-Replacement/Safeway Customer Order Import.TMS 12_06.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="19440" windowHeight="11700" tabRatio="725"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="19440" windowHeight="11700" tabRatio="725" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Customer Order Import" sheetId="19" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="ChangeLog_InternalUseOnly" sheetId="20" r:id="rId3"/>
     <sheet name="Terms and Conditions" sheetId="5" r:id="rId4"/>
     <sheet name="Sheet1" sheetId="22" r:id="rId5"/>
-    <sheet name="Payment Detail" sheetId="7" r:id="rId6"/>
+    <sheet name="RP_TO_EOM_MAPPING" sheetId="23" r:id="rId6"/>
+    <sheet name="Payment Detail" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Customer Order Import'!$A$6:$O$462</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Payment Detail'!$B$3:$F$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Payment Detail'!$B$3:$F$53</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -28,7 +29,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="I133" authorId="0">
+    <comment ref="I133" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3869,7 +3870,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="7">
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
@@ -4625,6 +4626,8 @@
     <xf numFmtId="0" fontId="23" fillId="8" borderId="1" xfId="53" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -4643,8 +4646,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="54">
     <cellStyle name="Comma  - Style1" xfId="7"/>
@@ -4715,6 +4716,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -4739,7 +4743,7 @@
         <xdr:cNvPr id="2" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4796,7 +4800,7 @@
         <xdr:cNvPr id="2" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4853,7 +4857,7 @@
         <xdr:cNvPr id="2" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4933,7 +4937,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4966,9 +4970,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5001,6 +5022,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -5180,11 +5218,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:EP476"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="L258" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="Q261" sqref="Q261"/>
+      <selection pane="bottomRight" activeCell="P258" sqref="P258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -11545,7 +11583,7 @@
         <v>1111</v>
       </c>
       <c r="M87" s="93"/>
-      <c r="N87" s="153" t="s">
+      <c r="N87" s="155" t="s">
         <v>1112</v>
       </c>
       <c r="O87" s="62" t="s">
@@ -11719,7 +11757,7 @@
         <v>1113</v>
       </c>
       <c r="M88" s="93"/>
-      <c r="N88" s="154"/>
+      <c r="N88" s="156"/>
       <c r="O88" s="62" t="s">
         <v>15</v>
       </c>
@@ -11891,7 +11929,7 @@
         <v>1114</v>
       </c>
       <c r="M89" s="93"/>
-      <c r="N89" s="155"/>
+      <c r="N89" s="157"/>
       <c r="O89" s="62" t="s">
         <v>15</v>
       </c>
@@ -20364,7 +20402,7 @@
       <c r="I257" s="148" t="s">
         <v>173</v>
       </c>
-      <c r="J257" s="159" t="s">
+      <c r="J257" s="153" t="s">
         <v>850</v>
       </c>
       <c r="K257" s="145" t="s">
@@ -20571,7 +20609,7 @@
       <c r="P261" s="152" t="s">
         <v>1185</v>
       </c>
-      <c r="Q261" s="160" t="s">
+      <c r="Q261" s="154" t="s">
         <v>1189</v>
       </c>
     </row>
@@ -32810,7 +32848,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -33489,6 +33527,18 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CJ56"/>
   <sheetViews>
@@ -33508,26 +33558,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:88" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="158" t="s">
+      <c r="B1" s="160" t="s">
         <v>976</v>
       </c>
-      <c r="C1" s="158"/>
-      <c r="D1" s="158"/>
-      <c r="E1" s="158"/>
-      <c r="F1" s="158"/>
+      <c r="C1" s="160"/>
+      <c r="D1" s="160"/>
+      <c r="E1" s="160"/>
+      <c r="F1" s="160"/>
       <c r="H1" s="48" t="s">
         <v>975</v>
       </c>
     </row>
     <row r="2" spans="1:88" s="3" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
-      <c r="B2" s="156" t="s">
+      <c r="B2" s="158" t="s">
         <v>743</v>
       </c>
-      <c r="C2" s="157"/>
-      <c r="D2" s="157"/>
-      <c r="E2" s="157"/>
-      <c r="F2" s="157"/>
+      <c r="C2" s="159"/>
+      <c r="D2" s="159"/>
+      <c r="E2" s="159"/>
+      <c r="F2" s="159"/>
       <c r="G2" s="2"/>
       <c r="H2" s="52" t="s">
         <v>744</v>
@@ -34799,6 +34849,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002173295A37465A41BF0BE8A78120550D" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="07edd680962e3b1259954c477d813847">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b2384c6cc0088fcedbaf6edaf557defa">
     <xsd:element name="properties">
@@ -34912,33 +34977,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E4A97CB-3B30-40EB-9DEC-ADDB553EE3E4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9ABEF02-4770-43B4-9B33-154D432D9B42}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -34959,9 +35001,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9ABEF02-4770-43B4-9B33-154D432D9B42}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E4A97CB-3B30-40EB-9DEC-ADDB553EE3E4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>